<commit_message>
updated codebase with final decided algo
</commit_message>
<xml_diff>
--- a/stock_list/mother_baby_stock.xlsx
+++ b/stock_list/mother_baby_stock.xlsx
@@ -138,14 +138,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF008000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -573,8 +573,8 @@
       <c r="L2" s="2">
         <v>57.75</v>
       </c>
-      <c r="M2" s="4">
-        <v>25.94</v>
+      <c r="M2" s="3">
+        <v>17.56</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -614,8 +614,8 @@
       <c r="L3" s="2">
         <v>70</v>
       </c>
-      <c r="M3" s="5">
-        <v>-28.69</v>
+      <c r="M3" s="4">
+        <v>-33.83</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -628,7 +628,7 @@
       <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>1114</v>
       </c>
       <c r="E4" s="2">
@@ -655,7 +655,7 @@
       <c r="L4" s="2">
         <v>1117.35</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="5">
         <v>156.56</v>
       </c>
     </row>
@@ -669,7 +669,7 @@
       <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>4163.85</v>
       </c>
       <c r="E5" s="2">
@@ -697,7 +697,7 @@
         <v>4239.4</v>
       </c>
       <c r="M5" s="3">
-        <v>18.93</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -710,7 +710,7 @@
       <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>184.15</v>
       </c>
       <c r="E6" s="2">
@@ -737,8 +737,8 @@
       <c r="L6" s="2">
         <v>186</v>
       </c>
-      <c r="M6" s="4">
-        <v>25.74</v>
+      <c r="M6" s="3">
+        <v>7.13</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -751,7 +751,7 @@
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>1782</v>
       </c>
       <c r="E7" s="2">
@@ -778,8 +778,8 @@
       <c r="L7" s="2">
         <v>1761.45</v>
       </c>
-      <c r="M7" s="4">
-        <v>48.48</v>
+      <c r="M7" s="5">
+        <v>20.03</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -792,7 +792,7 @@
       <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>3095.75</v>
       </c>
       <c r="E8" s="2">
@@ -819,8 +819,8 @@
       <c r="L8" s="2">
         <v>3006.3</v>
       </c>
-      <c r="M8" s="4">
-        <v>40.24</v>
+      <c r="M8" s="3">
+        <v>15.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>